<commit_message>
Deploying to gh-pages from  @ 2d347131359618a0d628192199d4951d39047522 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/3.b.1.xlsx
+++ b/en/downloads/data-excel/3.b.1.xlsx
@@ -71,9 +71,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Percentage of target population immunized with all vaccines included in national programs</t>
-  </si>
-  <si>
     <t>DTP vaccine coverage (for diphtheria, tetanus and pertussis) (3 doses)</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>(in percent)</t>
+  </si>
+  <si>
+    <t>3.b.1 Percentage of target population immunized with all vaccines included in national programs</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:T41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1449,24 +1449,24 @@
   <sheetData>
     <row r="1" spans="1:17" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>48</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -1503,13 +1503,13 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="C4" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>35</v>
       </c>
       <c r="D4" s="20">
         <v>2007</v>
@@ -1556,25 +1556,25 @@
     </row>
     <row r="5" spans="1:17" ht="36" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q5" s="52"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="21">
         <v>94.1</v>
@@ -1621,13 +1621,13 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="35" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="5">
         <v>93.4</v>
@@ -1674,13 +1674,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5">
         <v>93.6</v>
@@ -1727,13 +1727,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="5">
         <v>93.9</v>
@@ -1780,13 +1780,13 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="35" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5">
         <v>94.4</v>
@@ -1833,13 +1833,13 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5">
         <v>94.4</v>
@@ -1886,13 +1886,13 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="5">
         <v>94</v>
@@ -1939,13 +1939,13 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5">
         <v>94</v>
@@ -1992,13 +1992,13 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="5">
         <v>95</v>
@@ -2045,13 +2045,13 @@
     </row>
     <row r="15" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="37" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="6">
         <v>95.2</v>
@@ -2098,13 +2098,13 @@
     </row>
     <row r="16" spans="1:17" s="9" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -2122,13 +2122,13 @@
     </row>
     <row r="17" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="39">
         <v>98.8</v>
@@ -2175,13 +2175,13 @@
     </row>
     <row r="18" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="37" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="42">
         <v>99.2</v>
@@ -2228,13 +2228,13 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="45">
         <v>97.8</v>
@@ -2281,13 +2281,13 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="47">
         <v>99</v>
@@ -2334,13 +2334,13 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="35" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="45">
         <v>99.4</v>
@@ -2387,13 +2387,13 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="45">
         <v>98.9</v>
@@ -2440,13 +2440,13 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="45">
         <v>98.6</v>
@@ -2493,13 +2493,13 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" s="45">
         <v>99.1</v>
@@ -2546,13 +2546,13 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="45">
         <v>99.8</v>
@@ -2599,13 +2599,13 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" s="45">
         <v>98.8</v>
@@ -2652,13 +2652,13 @@
     </row>
     <row r="27" spans="1:19" ht="36" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2676,13 +2676,13 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>14</v>
@@ -2730,13 +2730,13 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="35" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>14</v>
@@ -2784,13 +2784,13 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="35" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>14</v>
@@ -2838,13 +2838,13 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>14</v>
@@ -2892,13 +2892,13 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="35" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>14</v>
@@ -2946,13 +2946,13 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>14</v>
@@ -3001,13 +3001,13 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>14</v>
@@ -3056,13 +3056,13 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>14</v>
@@ -3111,13 +3111,13 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>14</v>
@@ -3166,13 +3166,13 @@
     </row>
     <row r="37" spans="1:20" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="49" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>14</v>

</xml_diff>